<commit_message>
yashwantraut: hlookup and documentadd h and v lookup
</commit_message>
<xml_diff>
--- a/day-12 (2).xlsx
+++ b/day-12 (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data Analytics\Excel\ex 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BF2B7D-8C95-4D3A-B39D-E5149BD234B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9801FDB9-6AB5-4B5E-8E99-C58F97052A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,13 +222,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -268,7 +262,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,7 +668,7 @@
   <dimension ref="D4:N11"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="D5" sqref="D5:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -939,10 +932,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E4D76D-74B8-40DC-BEC8-E291CB4CB9A2}">
-  <dimension ref="C5:I17"/>
+  <dimension ref="C5:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:I6"/>
+      <selection activeCell="F9" sqref="D9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,209 +945,245 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="D6" s="6" t="str">
+        <f>HLOOKUP(D5,$C16:$I18,2,FALSE)</f>
+        <v>automotive sq, near tp road , 400001</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f t="shared" ref="E6:I6" si="0">HLOOKUP(E5,$C16:$I18,2,FALSE)</f>
+        <v>offline</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>2</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>1000</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>10000</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>6</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>7000</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>200000</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>1000</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="D9" s="6" t="str">
+        <f t="shared" ref="D9:E9" si="1">HLOOKUP(D5,$C16:$I18,3,FALSE)</f>
+        <v>nandanvan</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>online</v>
+      </c>
+      <c r="F9" s="6">
+        <f>HLOOKUP(F5,$C16:$I18,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="6">
+        <f>HLOOKUP(G5,$C16:$I18,3,FALSE)</f>
+        <v>15000</v>
+      </c>
+      <c r="H9" s="6">
+        <f>HLOOKUP(H5,$C16:$I18,3,FALSE)</f>
+        <v>200000</v>
+      </c>
+      <c r="I9" s="6">
+        <f>HLOOKUP(I5,$C16:$I18,3,FALSE)</f>
+        <v>5000</v>
+      </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>3</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>12000</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>150000</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>7000</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>10</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>2000</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>50000</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C15" s="6" t="s">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16" s="7" t="s">
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D17" s="6">
+        <v>700</v>
+      </c>
+      <c r="E17" s="6">
+        <v>100000</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="6">
+        <v>5000</v>
+      </c>
+      <c r="H17" s="6">
+        <v>5</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="7">
-        <v>100000</v>
-      </c>
-      <c r="G16" s="7">
-        <v>5</v>
-      </c>
-      <c r="H16" s="7">
-        <v>700</v>
-      </c>
-      <c r="I16" s="7">
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="6">
         <v>5000</v>
       </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="7">
-        <v>10000</v>
-      </c>
-      <c r="G17" s="7">
-        <v>2</v>
-      </c>
-      <c r="H17" s="7">
-        <v>100</v>
-      </c>
-      <c r="I17" s="7">
-        <v>1000</v>
+      <c r="E18" s="6">
+        <v>200000</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="6">
+        <v>15000</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>